<commit_message>
UPD 8 от 07.10.2021
- Разбил все показания на отдельные блоки,
- Сделал конфигуратор экрана в Excel,
- Отсортировал и поделил на группы переменные и функции,
- Добавил второй экран,
- Добавил блоки для отображения:
        * обороты (F),
        * уровень топлива (F),
        * EGT (F),
        * Давление масла (F).
</commit_message>
<xml_diff>
--- a/ADD/Конфигуратор_дисплея_128x64.xlsx
+++ b/ADD/Конфигуратор_дисплея_128x64.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8238" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8246" uniqueCount="43">
   <si>
     <t>.</t>
   </si>
@@ -115,9 +115,6 @@
     <t>УОЗ (H)</t>
   </si>
   <si>
-    <t>draw_fuel_f</t>
-  </si>
-  <si>
     <t>Израсходованное топливо (F)</t>
   </si>
   <si>
@@ -125,6 +122,33 @@
   </si>
   <si>
     <t>Скорость (F)</t>
+  </si>
+  <si>
+    <t>draw_rpm_f</t>
+  </si>
+  <si>
+    <t>Обороты (F)</t>
+  </si>
+  <si>
+    <t>draw_egt_f</t>
+  </si>
+  <si>
+    <t>EGT (F)</t>
+  </si>
+  <si>
+    <t>Уровень топлива (F)</t>
+  </si>
+  <si>
+    <t>Давление масла (F)</t>
+  </si>
+  <si>
+    <t>draw_fuel_tank_f</t>
+  </si>
+  <si>
+    <t>draw_fuel_burned_f</t>
+  </si>
+  <si>
+    <t>draw_oil_pressure_f</t>
   </si>
 </sst>
 </file>
@@ -367,16 +391,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -732,7 +756,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -786,7 +810,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -799,171 +823,171 @@
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="15" t="str">
+      <c r="B8" s="17" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(A1,Блоки!$A$2:$B$30,2,0),VLOOKUP(A8,Координаты!$A$2:$D$19,4,0),"    // ",A1),"")</f>
         <v xml:space="preserve">    draw_ff_fc_f(0, 0);    // Мгновенный расход топлива (F)</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="17" t="str">
+      <c r="B9" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(A2,Блоки!$A$2:$B$30,2,0),VLOOKUP(A9,Координаты!$A$2:$D$19,4,0),"    // ",A2),"")</f>
         <v/>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="17" t="str">
+      <c r="B10" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(A3,Блоки!$A$2:$B$30,2,0),VLOOKUP(A10,Координаты!$A$2:$D$19,4,0),"    // ",A3),"")</f>
         <v xml:space="preserve">    draw_water_temp_f(0, 22);    // Температура ОЖ (F)</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" s="17" t="str">
+      <c r="B11" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(A4,Блоки!$A$2:$B$30,2,0),VLOOKUP(A11,Координаты!$A$2:$D$19,4,0),"    // ",A4),"")</f>
         <v/>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="17" t="str">
+      <c r="B12" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(A5,Блоки!$A$2:$B$30,2,0),VLOOKUP(A12,Координаты!$A$2:$D$19,4,0),"    // ",A5),"")</f>
         <v xml:space="preserve">    draw_distance_f(0, 44);    // Суточный и общий пробег (F)</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
-      <c r="B13" s="17" t="str">
+      <c r="B13" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(A6,Блоки!$A$2:$B$30,2,0),VLOOKUP(A13,Координаты!$A$2:$D$19,4,0),"    // ",A6),"")</f>
         <v/>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
-      <c r="B14" s="17" t="str">
+      <c r="B14" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(B1,Блоки!$A$2:$B$30,2,0),VLOOKUP(A14,Координаты!$A$2:$D$19,4,0),"    // ",B1),"")</f>
         <v xml:space="preserve">    draw_map_h(43, 0);    // ДАД (H)</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
-      <c r="B15" s="17" t="str">
+      <c r="B15" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(B2,Блоки!$A$2:$B$30,2,0),VLOOKUP(A15,Координаты!$A$2:$D$19,4,0),"    // ",B2),"")</f>
         <v xml:space="preserve">    draw_airtemp_h(43, 10);    // Температура воздуха на впуске (H)</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
-      <c r="B16" s="17" t="str">
+      <c r="B16" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(B3,Блоки!$A$2:$B$30,2,0),VLOOKUP(A16,Координаты!$A$2:$D$19,4,0),"    // ",B3),"")</f>
         <v xml:space="preserve">    draw_trottle_f(43, 22);    // ДПДЗ / РХХ (F)</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="B17" s="17" t="str">
+      <c r="B17" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(B4,Блоки!$A$2:$B$30,2,0),VLOOKUP(A17,Координаты!$A$2:$D$19,4,0),"    // ",B4),"")</f>
         <v/>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
-      <c r="B18" s="17" t="str">
+      <c r="B18" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(B5,Блоки!$A$2:$B$30,2,0),VLOOKUP(A18,Координаты!$A$2:$D$19,4,0),"    // ",B5),"")</f>
         <v xml:space="preserve">    draw_afc_f(43, 44);    // Средний расход топлива (F)</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>
-      <c r="B19" s="17" t="str">
+      <c r="B19" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(B6,Блоки!$A$2:$B$30,2,0),VLOOKUP(A19,Координаты!$A$2:$D$19,4,0),"    // ",B6),"")</f>
         <v/>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>13</v>
       </c>
-      <c r="B20" s="17" t="str">
+      <c r="B20" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(C1,Блоки!$A$2:$B$30,2,0),VLOOKUP(A20,Координаты!$A$2:$D$19,4,0),"    // ",C1),"")</f>
         <v xml:space="preserve">    draw_O2_sensor_h(86, 0);    // Напряжение УДК / AFR (H)</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>14</v>
       </c>
-      <c r="B21" s="17" t="str">
+      <c r="B21" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(C2,Блоки!$A$2:$B$30,2,0),VLOOKUP(A21,Координаты!$A$2:$D$19,4,0),"    // ",C2),"")</f>
         <v xml:space="preserve">    draw_lambda_corr_h(86, 10);    // Лямбда коррекция (H)</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>15</v>
       </c>
-      <c r="B22" s="17" t="str">
+      <c r="B22" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(C3,Блоки!$A$2:$B$30,2,0),VLOOKUP(A22,Координаты!$A$2:$D$19,4,0),"    // ",C3),"")</f>
         <v xml:space="preserve">    draw_battery_h(86, 22);    // Напряжение сети (H)</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>16</v>
       </c>
-      <c r="B23" s="17" t="str">
+      <c r="B23" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(C4,Блоки!$A$2:$B$30,2,0),VLOOKUP(A23,Координаты!$A$2:$D$19,4,0),"    // ",C4),"")</f>
         <v xml:space="preserve">    draw_angle_h(86, 32);    // УОЗ (H)</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>17</v>
       </c>
-      <c r="B24" s="17" t="str">
+      <c r="B24" s="15" t="str">
         <f>IFERROR(CONCATENATE("    ",VLOOKUP(C5,Блоки!$A$2:$B$30,2,0),VLOOKUP(A24,Координаты!$A$2:$D$19,4,0),"    // ",C5),"")</f>
-        <v xml:space="preserve">    draw_fuel_f(86, 44);    // Израсходованное топливо (F)</v>
-      </c>
-      <c r="C24" s="18"/>
+        <v xml:space="preserve">    draw_fuel_burned_f(86, 44);    // Израсходованное топливо (F)</v>
+      </c>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -977,11 +1001,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -989,12 +1008,17 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:C2">
     <cfRule type="expression" dxfId="5" priority="5">
@@ -1039,11 +1063,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1062,119 +1084,151 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1">
-    <sortState ref="A2:B14">
+    <sortState ref="A2:B19">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>